<commit_message>
Well, it's updated to the new .csproj format....
</commit_message>
<xml_diff>
--- a/Statistics.xlsx
+++ b/Statistics.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Code Base</t>
   </si>
@@ -97,12 +97,27 @@
   </si>
   <si>
     <t>MSBuild Difference</t>
+  </si>
+  <si>
+    <t>The AngleSharp + NodaTime MSBuild test took 02:16:21</t>
+  </si>
+  <si>
+    <t>SyntaxFactory Tab Speed</t>
+  </si>
+  <si>
+    <t>SyntaxFactory Spaces Speed</t>
+  </si>
+  <si>
+    <t>SyntaxFactory Difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,8 +147,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,12 +441,13 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -574,133 +599,459 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="178" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="20.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="178" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>13.276400000000001</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>13.3497</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2">
+        <v>7.3564999999999996</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7.4688999999999997</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2.5514000000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>2.5596000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>4.8895</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4.9175000000000004</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
+        <v>1.1837</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B4" s="2">
+        <v>0.78853119999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.78819079999999997</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1">
+        <v>3.1737000000000002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3.1589999999999998</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>0.68990649999999998</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.6561593</v>
+      </c>
+      <c r="J4" s="3">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="K4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
+      <c r="B5" s="2">
+        <v>1.5561475</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.5624929000000001</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>4.6066000000000003</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4.7074999999999996</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>1.2880039000000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.2998299</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>3.2050000000000001</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>3.1924999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>2.5943999999999998</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.5964999999999998</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>2.6856946000000002</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2.6646904</v>
+      </c>
+      <c r="J6" s="3">
+        <v>-0.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="H7" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>8.3787000000000003</v>
+      </c>
+      <c r="F7" s="2">
+        <v>8.4435000000000002</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>0.77562790000000004</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.79219830000000002</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.09</v>
+      </c>
+      <c r="K7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>7.2492000000000001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>7.3002000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>6.875</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6.9550999999999998</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>2.2037958</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2.2334839</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>4.0263999999999998</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>4.0599999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>2.9419</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2.9357000000000002</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>1.2187759</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.2123463000000001</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" t="s">
+      <c r="B10" s="2">
+        <v>1.7329201000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.7426619000000001</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>3.5981999999999998</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.5977999999999999</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>1.5704254</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.5763384</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="K10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7.3564999999999996</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7.4688999999999997</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.1837</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.68990649999999998</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.6561593</v>
+      </c>
+      <c r="D18" s="3">
+        <v>-4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.2880039000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.2998299</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.6856946000000002</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.6646904</v>
+      </c>
+      <c r="D20" s="3">
+        <v>-0.78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.77562790000000004</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.79219830000000002</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2.2037958</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2.2334839</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.2187759</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.2123463000000001</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.5704254</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.5763384</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>